<commit_message>
picture - delete, update room - main 화면 및 관련 작업들
</commit_message>
<xml_diff>
--- a/data/docs/csv/room 전체 툴.xlsx
+++ b/data/docs/csv/room 전체 툴.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KHRDI-05\Desktop\project_hotel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\workspace-jsp\project_hotel\data\docs\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12288"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
   <si>
     <t>상세이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -111,10 +111,6 @@
   </si>
   <si>
     <t>바다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>트윈</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -195,7 +191,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -575,19 +571,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.59765625" style="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
     <col min="6" max="6" width="9.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -601,38 +597,38 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -647,12 +643,12 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
@@ -667,12 +663,12 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -687,12 +683,12 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
@@ -707,7 +703,7 @@
         <v>280000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -721,14 +717,13 @@
         <v>40</v>
       </c>
       <c r="E7" s="1">
-        <f>E6+2</f>
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F7" s="1">
         <v>313000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -742,14 +737,13 @@
         <v>40</v>
       </c>
       <c r="E8" s="1">
-        <f>E7+2</f>
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="F8" s="1">
         <v>313000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
@@ -763,14 +757,13 @@
         <v>40</v>
       </c>
       <c r="E9" s="1">
-        <f>E8+2</f>
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="F9" s="1">
         <v>313000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
@@ -784,19 +777,18 @@
         <v>40</v>
       </c>
       <c r="E10" s="1">
-        <f>E9+2</f>
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F10" s="1">
         <v>313000</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>12</v>
@@ -811,12 +803,12 @@
         <v>313000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>12</v>
@@ -831,12 +823,12 @@
         <v>313000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
@@ -845,19 +837,18 @@
         <v>40</v>
       </c>
       <c r="E13" s="1">
-        <f>E12+2</f>
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F13" s="1">
         <v>313000</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
@@ -866,19 +857,18 @@
         <v>40</v>
       </c>
       <c r="E14" s="1">
-        <f>E13+2</f>
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="F14" s="1">
         <v>313000</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>12</v>
@@ -887,19 +877,18 @@
         <v>40</v>
       </c>
       <c r="E15" s="1">
-        <f>E14+2</f>
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="F15" s="1">
         <v>403000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>12</v>
@@ -908,19 +897,18 @@
         <v>40</v>
       </c>
       <c r="E16" s="1">
-        <f>E15+2</f>
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="F16" s="1">
         <v>403000</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>11</v>
@@ -929,19 +917,18 @@
         <v>40</v>
       </c>
       <c r="E17" s="1">
-        <f>E16+2</f>
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="F17" s="1">
         <v>403000</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>11</v>
@@ -950,14 +937,13 @@
         <v>40</v>
       </c>
       <c r="E18" s="1">
-        <f>E17+2</f>
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="F18" s="1">
         <v>403000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" s="2" t="s">
         <v>13</v>
       </c>
@@ -977,7 +963,7 @@
         <v>385000</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -997,7 +983,7 @@
         <v>385000</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" s="2" t="s">
         <v>13</v>
       </c>
@@ -1011,14 +997,13 @@
         <v>40</v>
       </c>
       <c r="E21" s="1">
-        <f>E20+2</f>
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F21" s="1">
         <v>360000</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
@@ -1032,14 +1017,13 @@
         <v>40</v>
       </c>
       <c r="E22" s="1">
-        <f>E21+2</f>
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F22" s="1">
         <v>360000</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
@@ -1053,14 +1037,13 @@
         <v>40</v>
       </c>
       <c r="E23" s="1">
-        <f>E22+2</f>
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F23" s="1">
         <v>360000</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
@@ -1074,14 +1057,13 @@
         <v>40</v>
       </c>
       <c r="E24" s="1">
-        <f>E23+2</f>
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="F24" s="1">
         <v>360000</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1101,7 +1083,7 @@
         <v>329000</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>6</v>
       </c>
@@ -1109,7 +1091,7 @@
         <v>17</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D26" s="2">
         <v>46</v>
@@ -1121,7 +1103,7 @@
         <v>329000</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1129,20 +1111,19 @@
         <v>10</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D27" s="2">
         <v>46</v>
       </c>
       <c r="E27" s="1">
-        <f>E26+2</f>
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F27" s="1">
         <v>445000</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -1156,14 +1137,13 @@
         <v>46</v>
       </c>
       <c r="E28" s="1">
-        <f>E27+2</f>
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="F28" s="1">
         <v>445000</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" s="2" t="s">
         <v>18</v>
       </c>
@@ -1177,14 +1157,13 @@
         <v>46</v>
       </c>
       <c r="E29" s="1">
-        <f>E26+2</f>
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="F29" s="1">
         <v>510000</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" s="2" t="s">
         <v>18</v>
       </c>
@@ -1204,7 +1183,7 @@
         <v>510000</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
@@ -1224,7 +1203,7 @@
         <v>1080000</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" s="2" t="s">
         <v>20</v>
       </c>
@@ -1232,7 +1211,7 @@
         <v>7</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D32" s="2">
         <v>72</v>
@@ -1244,7 +1223,7 @@
         <v>1080000</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" s="2" t="s">
         <v>20</v>
       </c>
@@ -1252,7 +1231,7 @@
         <v>21</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D33" s="2">
         <v>72</v>
@@ -1264,7 +1243,7 @@
         <v>980000</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>20</v>
       </c>
@@ -1284,15 +1263,15 @@
         <v>980000</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="D35" s="2">
         <v>158</v>
@@ -1304,15 +1283,15 @@
         <v>7200000</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D36" s="2">
         <v>277</v>

</xml_diff>